<commit_message>
move files for trxn map
</commit_message>
<xml_diff>
--- a/Cust-Trxn-Channel-Charts/scratch/dataframe copy.xlsx
+++ b/Cust-Trxn-Channel-Charts/scratch/dataframe copy.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DataFrame" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -488,7 +488,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -508,7 +508,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -528,7 +528,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -548,7 +548,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -588,7 +588,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -608,7 +608,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -628,7 +628,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -643,15 +643,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Nan</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
+          <t>Payments</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.474</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -661,16 +663,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Payments</t>
+          <t>Billing</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Billing</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4.474</v>
+        <v>1.241</v>
       </c>
     </row>
     <row r="13">
@@ -681,16 +683,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Billing</t>
+          <t>Pay Plans</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Pay Plans</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1.241</v>
+        <v>0.209</v>
       </c>
     </row>
     <row r="14">
@@ -701,16 +703,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Pay Plans</t>
+          <t>Account Balance</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Account Balance</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.209</v>
+        <v>0.205</v>
       </c>
     </row>
     <row r="15">
@@ -721,16 +723,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Account Balance</t>
+          <t>Start/Stop/ Transfer</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Start</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.205</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="16">
@@ -746,10 +748,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Nan</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
+          <t>Stop</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.124</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -764,11 +768,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Start </t>
+          <t>Transfer</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.155</v>
+        <v>0.058</v>
       </c>
     </row>
     <row r="18">
@@ -779,16 +783,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Outage</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stop </t>
+          <t>Outage</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.124</v>
+        <v>0.843</v>
       </c>
     </row>
     <row r="19">
@@ -799,96 +803,96 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Other Transactions</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Transfer </t>
+          <t>Other Transactions</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.058</v>
+        <v>0.678</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Call Center IVR</t>
+          <t>Call Center Other</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Outage </t>
+          <t>ICM Technology Handled1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Icm Technology Handled1</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.843</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Call Center IVR</t>
+          <t>Call Center Other</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Other Transactions </t>
+          <t>NonIVR Technology2</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Nonivr Technology2</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.678</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Call Center Other</t>
+          <t>Call CenterLive Agent</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ICM Technology Handled1</t>
+          <t>Handled calls</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Handled Calls</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2.63</v>
+        <v>5.242</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Call Center Other</t>
+          <t>Call CenterLive Agent</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NonIVR Technology2</t>
+          <t>Transferred calls4</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Transferred Calls4</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.029</v>
+        <v>3.918</v>
       </c>
     </row>
     <row r="24">
@@ -899,15 +903,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Live Agent </t>
+          <t>Abandoned Calls</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Nan</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
+          <t>Abandoned Calls</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.267</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -917,16 +923,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Handled calls </t>
+          <t>General</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>General</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>5.242</v>
+        <v>1.341</v>
       </c>
     </row>
     <row r="26">
@@ -937,16 +943,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Transferred calls4 </t>
+          <t>Billing Balance</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Billing Balance</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.918</v>
+        <v>0.6909999999999999</v>
       </c>
     </row>
     <row r="27">
@@ -957,16 +963,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Abandoned Calls</t>
+          <t>Start/Stop/ Transfer</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Start</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.267</v>
+        <v>0.374</v>
       </c>
     </row>
     <row r="28">
@@ -977,16 +983,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>General</t>
+          <t>Start/Stop/ Transfer</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Stop</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1.341</v>
+        <v>0.133</v>
       </c>
     </row>
     <row r="29">
@@ -997,16 +1003,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Billing Balance </t>
+          <t>Start/Stop/ Transfer</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Transfer</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.171</v>
       </c>
     </row>
     <row r="30">
@@ -1017,15 +1023,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>BCSC (Business Customer Service Center)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Nan</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
+          <t>Bcsc (Business Customer Service Center)</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0.466</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1035,16 +1043,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Emergency</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Start </t>
+          <t>Emergency</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.374</v>
+        <v>0.449</v>
       </c>
     </row>
     <row r="32">
@@ -1055,16 +1063,16 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Outage</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stop </t>
+          <t>Outage</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.133</v>
+        <v>0.246</v>
       </c>
     </row>
     <row r="33">
@@ -1075,16 +1083,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Spanish (General)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Transfer </t>
+          <t>Spanish (General)</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.171</v>
+        <v>0.256</v>
       </c>
     </row>
     <row r="34">
@@ -1095,16 +1103,16 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BCSC (Business Customer Service Center)</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.466</v>
+        <v>0.137</v>
       </c>
     </row>
     <row r="35">
@@ -1115,16 +1123,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Emergency </t>
+          <t>Solar</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Solar</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.449</v>
+        <v>0.479</v>
       </c>
     </row>
     <row r="36">
@@ -1135,16 +1143,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Outage </t>
+          <t>Specialty Lines</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Specialty Lines</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.246</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="37">
@@ -1155,16 +1163,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Spanish (General) </t>
+          <t>Pay Plans</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Pay Plans</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.256</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="38">
@@ -1175,96 +1183,96 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Payments</t>
+          <t>Other Transactions</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Other Transactions</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.137</v>
+        <v>0.136</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Call CenterLive Agent</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Solar </t>
+          <t>Payment</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Payment</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.479</v>
+        <v>27.950047</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Call CenterLive Agent</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Specialty Lines </t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>One Time Access</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.22</v>
+        <v>3.633827</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Call CenterLive Agent</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Pay Plans</t>
+          <t>Payments</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Your Account</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.123</v>
+        <v>24.31622</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Call CenterLive Agent</t>
+          <t>Web</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Other Transactions </t>
+          <t>Billing</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Billing</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.136</v>
+        <v>18.35347</v>
       </c>
     </row>
     <row r="43">
@@ -1275,15 +1283,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>ViewBillCurrentPDF</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Nan</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr"/>
+          <t>Viewbillcurrentpdf</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>8.992262999999999</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1293,16 +1303,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Payment</t>
+          <t>ViewBillCurrentPDF historical</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Viewbillcurrentpdf Historical</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>27.950047</v>
+        <v>9.361207</v>
       </c>
     </row>
     <row r="45">
@@ -1313,16 +1323,16 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Payments</t>
+          <t>Usage and Rates</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>One Time Access</t>
+          <t>Usage And Rates</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>3.633827</v>
+        <v>6.742749</v>
       </c>
     </row>
     <row r="46">
@@ -1333,16 +1343,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Payments</t>
+          <t>Usage and Rates</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Your Account</t>
+          <t>View Usage</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>24.31622</v>
+        <v>3.193489</v>
       </c>
     </row>
     <row r="47">
@@ -1353,16 +1363,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Billing</t>
+          <t>Usage and Rates</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Compare My Bills</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>18.35347</v>
+        <v>2.735761</v>
       </c>
     </row>
     <row r="48">
@@ -1373,16 +1383,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ViewBillCurrentPDF</t>
+          <t>Usage and Rates</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Viewbillcurrentpdf</t>
+          <t>Rate Comparison</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>8.992262999999999</v>
+        <v>0.310259</v>
       </c>
     </row>
     <row r="49">
@@ -1393,16 +1403,16 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ViewBillCurrentPDF historical</t>
+          <t>Usage and Rates</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Viewbillcurrentpdf Historical</t>
+          <t>Home Energy Checkup</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>9.361207</v>
+        <v>0.36242</v>
       </c>
     </row>
     <row r="50">
@@ -1418,11 +1428,11 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Online Rate Enrollment</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>6.742749</v>
+        <v>0.14082</v>
       </c>
     </row>
     <row r="51">
@@ -1433,16 +1443,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Usage and Rates</t>
+          <t>Outage</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t xml:space="preserve">View Usage </t>
+          <t>Outage</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>3.193489</v>
+        <v>5.146001</v>
       </c>
     </row>
     <row r="52">
@@ -1453,16 +1463,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Usage and Rates</t>
+          <t>Outage</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Compare My Bills</t>
+          <t>Report Outage</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2.735761</v>
+        <v>0.549793</v>
       </c>
     </row>
     <row r="53">
@@ -1473,16 +1483,16 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Usage and Rates</t>
+          <t>Outage</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Rate Comparison</t>
+          <t>Search Outage By Address</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.310259</v>
+        <v>4.516009</v>
       </c>
     </row>
     <row r="54">
@@ -1493,16 +1503,16 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Usage and Rates</t>
+          <t>Outage</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Home Energy Checkup</t>
+          <t>Subscribe Outage (Ew Pages)</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.36242</v>
+        <v>0.08019900000000001</v>
       </c>
     </row>
     <row r="55">
@@ -1513,16 +1523,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Usage and Rates</t>
+          <t>Account Mgmt</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Online Rate Enrollment</t>
+          <t>Account Mgmt</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.14082</v>
+        <v>0.381154</v>
       </c>
     </row>
     <row r="56">
@@ -1533,16 +1543,16 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Outage</t>
+          <t>Account Mgmt</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Change Billing Address</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>5.146001</v>
+        <v>0.08394699999999999</v>
       </c>
     </row>
     <row r="57">
@@ -1553,16 +1563,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Outage</t>
+          <t>Account Mgmt</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Report Outage</t>
+          <t>Add/Edit Phone Number</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.549793</v>
+        <v>0.1376</v>
       </c>
     </row>
     <row r="58">
@@ -1573,16 +1583,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Outage</t>
+          <t>Account Mgmt</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Search Outage By Address</t>
+          <t>Change User Name, Password</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>4.516009</v>
+        <v>0.159607</v>
       </c>
     </row>
     <row r="59">
@@ -1593,16 +1603,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Outage</t>
+          <t>Payment Account NEW</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Subscribe Outage (Ew Pages)</t>
+          <t>Payment Account New</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.08019900000000001</v>
+        <v>0.923619</v>
       </c>
     </row>
     <row r="60">
@@ -1613,16 +1623,16 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Account Mgmt</t>
+          <t>Payment Account NEW</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Create_Payment_Account</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.381154</v>
+        <v>0.663126</v>
       </c>
     </row>
     <row r="61">
@@ -1633,16 +1643,16 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Account Mgmt</t>
+          <t>Payment Account NEW</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Change Billing Address </t>
+          <t>Update_Payment_Account</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.08394699999999999</v>
+        <v>0.016176</v>
       </c>
     </row>
     <row r="62">
@@ -1653,16 +1663,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Account Mgmt</t>
+          <t>Payment Account NEW</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Add/Edit Phone Number</t>
+          <t>Delete_Payment_Account</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.1376</v>
+        <v>0.244317</v>
       </c>
     </row>
     <row r="63">
@@ -1673,16 +1683,16 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Account Mgmt</t>
+          <t>Start/Stop/ Transfer</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Change User Name, Password </t>
+          <t>Start</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.159607</v>
+        <v>0.200864</v>
       </c>
     </row>
     <row r="64">
@@ -1693,16 +1703,16 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Payment Account NEW</t>
+          <t>Start/Stop/ Transfer</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Start</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.923619</v>
+        <v>0.08201899999999999</v>
       </c>
     </row>
     <row r="65">
@@ -1713,16 +1723,16 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Payment Account NEW</t>
+          <t>Start/Stop/ Transfer</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Create_Payment_Account</t>
+          <t>Stop</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.663126</v>
+        <v>0.178445</v>
       </c>
     </row>
     <row r="66">
@@ -1733,16 +1743,16 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Payment Account NEW</t>
+          <t>Start/Stop/ Transfer</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Update_Payment_Account</t>
+          <t>Transfer</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.016176</v>
+        <v>0.08018699999999999</v>
       </c>
     </row>
     <row r="67">
@@ -1753,16 +1763,16 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Payment Account NEW</t>
+          <t>Pay Plans</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Delete_Payment_Account</t>
+          <t>Pay Plans</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.244317</v>
+        <v>0.300009</v>
       </c>
     </row>
     <row r="68">
@@ -1773,15 +1783,17 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Pay Plans</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Nan</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr"/>
+          <t>Installment Pay</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>0.220049</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1791,15 +1803,17 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Pay Plans</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Start </t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr"/>
+          <t>Extension Pay</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>0.07996</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1809,16 +1823,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>CARE/FERA</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Start </t>
+          <t>Care/Fera</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.200864</v>
+        <v>0.278569</v>
       </c>
     </row>
     <row r="71">
@@ -1829,16 +1843,16 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Alerts &amp; Notifications</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Start </t>
+          <t>Alerts &amp; Notifications</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.08201899999999999</v>
+        <v>0.6301449999999998</v>
       </c>
     </row>
     <row r="72">
@@ -1849,16 +1863,16 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Alerts &amp; Notifications</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stop </t>
+          <t>Change Billing &amp; Payment Alerts</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.178445</v>
+        <v>0.30238</v>
       </c>
     </row>
     <row r="73">
@@ -1869,16 +1883,16 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Start/Stop/ Transfer</t>
+          <t>Alerts &amp; Notifications</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Transfer </t>
+          <t>Energy Alerts</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.08018699999999999</v>
+        <v>0.233548</v>
       </c>
     </row>
     <row r="74">
@@ -1889,16 +1903,16 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Pay Plans</t>
+          <t>Alerts &amp; Notifications</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Outages Alerts New</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.300009</v>
+        <v>0.012242</v>
       </c>
     </row>
     <row r="75">
@@ -1909,16 +1923,16 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Pay Plans</t>
+          <t>Alerts &amp; Notifications</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Installment Pay</t>
+          <t>Go Paperless Alerts New</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.220049</v>
+        <v>0.025758</v>
       </c>
     </row>
     <row r="76">
@@ -1929,16 +1943,16 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Pay Plans</t>
+          <t>Alerts &amp; Notifications</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Extension Pay</t>
+          <t>Notices &amp; Services Information New</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.07996</v>
+        <v>0.010738</v>
       </c>
     </row>
     <row r="77">
@@ -1949,16 +1963,16 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t xml:space="preserve">CARE/FERA </t>
+          <t>Alerts &amp; Notifications</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Event Day Alerts New</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.278569</v>
+        <v>0.016104</v>
       </c>
     </row>
     <row r="78">
@@ -1974,11 +1988,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Service Visit Alerts New</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.6301449999999998</v>
+        <v>0.003697</v>
       </c>
     </row>
     <row r="79">
@@ -1994,11 +2008,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Change Billing &amp; Payment Alerts </t>
+          <t>Additional Communication Alerts New</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.30238</v>
+        <v>0.008685999999999999</v>
       </c>
     </row>
     <row r="80">
@@ -2014,11 +2028,11 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Energy Alerts</t>
+          <t>Pay Plan &amp; Shutoff Nonpayment Alerts New</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.233548</v>
+        <v>0.016992</v>
       </c>
     </row>
     <row r="81">
@@ -2029,16 +2043,16 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications</t>
+          <t>Pilot Light Appointments</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Outages Alerts New</t>
+          <t>Pilot Light Appointments</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.012242</v>
+        <v>0.022042</v>
       </c>
     </row>
     <row r="82">
@@ -2049,16 +2063,16 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications</t>
+          <t>Pilot Light Appointments</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Go Paperless Alerts New</t>
+          <t>Schedule_Service_Appointment</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.025758</v>
+        <v>0.018987</v>
       </c>
     </row>
     <row r="83">
@@ -2069,16 +2083,16 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications</t>
+          <t>Pilot Light Appointments</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Notices &amp; Services Information New</t>
+          <t>Reschedule_Service_Appointment</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.010738</v>
+        <v>0.001148</v>
       </c>
     </row>
     <row r="84">
@@ -2089,16 +2103,16 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications</t>
+          <t>Pilot Light Appointments</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Event Day Alerts New</t>
+          <t>Cancel_Service_Appointment</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.016104</v>
+        <v>0.001907</v>
       </c>
     </row>
     <row r="85">
@@ -2109,16 +2123,16 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications</t>
+          <t>Budget Billing (Login)</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Service Visit Alerts New</t>
+          <t>Budget Billing (Login)</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0.003697</v>
+        <v>0.016692</v>
       </c>
     </row>
     <row r="86">
@@ -2129,16 +2143,16 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications</t>
+          <t>Other Interactions</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Additional Communication Alerts New</t>
+          <t>Other Interactions</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.008685999999999999</v>
+        <v>1.310914</v>
       </c>
     </row>
     <row r="87">
@@ -2149,16 +2163,16 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Alerts &amp; Notifications</t>
+          <t>Other Interactions</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Pay Plan &amp; Shutoff Nonpayment Alerts New</t>
+          <t>Gas Pipeline Map Views</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.016992</v>
+        <v>0.015393</v>
       </c>
     </row>
     <row r="88">
@@ -2169,16 +2183,16 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pilot Light Appointments </t>
+          <t>Other Interactions</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Nan</t>
+          <t>Recurring Payment Schedule</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0.022042</v>
+        <v>0.7567469999999999</v>
       </c>
     </row>
     <row r="89">
@@ -2189,173 +2203,15 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pilot Light Appointments </t>
+          <t>Other Interactions</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Schedule_Service_Appointment</t>
+          <t>Registration</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0.018987</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Pilot Light Appointments </t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Reschedule_Service_Appointment</t>
-        </is>
-      </c>
-      <c r="D90" t="n">
-        <v>0.001148</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Pilot Light Appointments </t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Cancel_Service_Appointment</t>
-        </is>
-      </c>
-      <c r="D91" t="n">
-        <v>0.001907</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Budget Billing (Login) </t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Nan</t>
-        </is>
-      </c>
-      <c r="D92" t="n">
-        <v>0.016692</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Other Interactions </t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Nan</t>
-        </is>
-      </c>
-      <c r="D93" t="n">
-        <v>1.310914</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Other Interactions </t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Gas Pipeline Map Views</t>
-        </is>
-      </c>
-      <c r="D94" t="n">
-        <v>0.015393</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Other Interactions </t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Contact Us</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr"/>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Other Interactions </t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>Recurring Payment Schedule</t>
-        </is>
-      </c>
-      <c r="D96" t="n">
-        <v>0.7567469999999999</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>Web</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Other Interactions </t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>Registration</t>
-        </is>
-      </c>
-      <c r="D97" t="n">
         <v>0.538774</v>
       </c>
     </row>

</xml_diff>